<commit_message>
[unc-ebike] add spanish translations
</commit_message>
<xml_diff>
--- a/survey_resources/unc-ebike/onboarding-v1.xlsx
+++ b/survey_resources/unc-ebike/onboarding-v1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11013"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mwbc/git/nrel-openpath-deploy-configs/survey_resources/unc-ebike/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{69B37E78-19AF-9F4D-84E0-718B258C51AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0C2AB46-7DD2-EF48-9F7D-6480590DB6D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2140" yWindow="2380" windowWidth="23640" windowHeight="10720" activeTab="1" xr2:uid="{0DB3CBBC-5CBF-ED4D-ACA3-54E53E9C3B9D}"/>
+    <workbookView xWindow="2140" yWindow="2380" windowWidth="23640" windowHeight="10720" xr2:uid="{0DB3CBBC-5CBF-ED4D-ACA3-54E53E9C3B9D}"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -57,9 +57,6 @@
     <t>What type of smartphone do you have?</t>
   </si>
   <si>
-    <t>¿Que tipo de teléfono inteligente usted tiene?</t>
-  </si>
-  <si>
     <t>list_name</t>
   </si>
   <si>
@@ -84,16 +81,19 @@
     <t>Don't know</t>
   </si>
   <si>
-    <t>No lo sé</t>
-  </si>
-  <si>
     <t>other</t>
   </si>
   <si>
     <t>Other</t>
   </si>
   <si>
-    <t>Otro tipo</t>
+    <t>No sé</t>
+  </si>
+  <si>
+    <t>Otro</t>
+  </si>
+  <si>
+    <t>¿Qué tipo de teléfono inteligente usas?</t>
   </si>
 </sst>
 </file>
@@ -129,8 +129,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -467,8 +470,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FCF4B551-F8E1-DF49-969A-C3B2643D54E0}">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -484,10 +487,10 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="68" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -497,8 +500,8 @@
       <c r="C2" t="s">
         <v>5</v>
       </c>
-      <c r="D2" t="s">
-        <v>6</v>
+      <c r="D2" s="1" t="s">
+        <v>18</v>
       </c>
     </row>
   </sheetData>
@@ -510,8 +513,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7CA3A6AF-0463-A849-96CC-F5CCE837BEFB}">
   <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -522,7 +525,7 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
@@ -531,7 +534,7 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -539,13 +542,13 @@
         <v>4</v>
       </c>
       <c r="B2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" t="s">
         <v>9</v>
       </c>
-      <c r="C2" t="s">
-        <v>10</v>
-      </c>
       <c r="D2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -553,13 +556,13 @@
         <v>4</v>
       </c>
       <c r="B3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" t="s">
         <v>11</v>
       </c>
-      <c r="C3" t="s">
-        <v>12</v>
-      </c>
       <c r="D3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
@@ -567,13 +570,13 @@
         <v>4</v>
       </c>
       <c r="B4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" t="s">
         <v>13</v>
       </c>
-      <c r="C4" t="s">
-        <v>14</v>
-      </c>
       <c r="D4" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
@@ -581,13 +584,13 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D5" t="s">
         <v>17</v>
-      </c>
-      <c r="D5" t="s">
-        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>